<commit_message>
push updated time plan
</commit_message>
<xml_diff>
--- a/doc/Time Tracking/Time Sheet.xlsx
+++ b/doc/Time Tracking/Time Sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vivek\Desktop\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vivek\Desktop\Project\pg-scrambLe.git\doc\Time Tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -240,6 +240,19 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -252,19 +265,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:V39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,29 +560,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="19"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="17"/>
     </row>
     <row r="3" spans="2:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
@@ -630,11 +630,11 @@
         <v>0</v>
       </c>
       <c r="C4" s="10"/>
-      <c r="D4" s="20"/>
+      <c r="D4" s="13"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -655,11 +655,11 @@
         <v>7</v>
       </c>
       <c r="C5" s="10"/>
-      <c r="D5" s="20"/>
+      <c r="D5" s="13"/>
       <c r="E5" s="10"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -680,11 +680,11 @@
         <v>1</v>
       </c>
       <c r="C6" s="10"/>
-      <c r="D6" s="20"/>
+      <c r="D6" s="13"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -705,11 +705,11 @@
         <v>2</v>
       </c>
       <c r="C7" s="10"/>
-      <c r="D7" s="20"/>
+      <c r="D7" s="13"/>
       <c r="E7" s="10"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -730,11 +730,11 @@
         <v>3</v>
       </c>
       <c r="C8" s="10"/>
-      <c r="D8" s="20"/>
+      <c r="D8" s="13"/>
       <c r="E8" s="12"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -755,11 +755,11 @@
         <v>4</v>
       </c>
       <c r="C9" s="10"/>
-      <c r="D9" s="20"/>
+      <c r="D9" s="13"/>
       <c r="E9" s="10"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -780,11 +780,11 @@
         <v>5</v>
       </c>
       <c r="C10" s="10"/>
-      <c r="D10" s="20"/>
+      <c r="D10" s="13"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -805,11 +805,11 @@
         <v>6</v>
       </c>
       <c r="C11" s="10"/>
-      <c r="D11" s="20"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="10"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -844,14 +844,14 @@
       </c>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
@@ -866,152 +866,152 @@
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="15"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="20"/>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="15"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="20"/>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="15"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="20"/>
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="15"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="20"/>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="15"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="20"/>
     </row>
     <row r="28" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="15"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="20"/>
     </row>
     <row r="29" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="15"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="20"/>
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="15"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="20"/>
     </row>
     <row r="31" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C31" s="1"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="15"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="20"/>
     </row>
     <row r="32" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C32" s="1"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="15"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="20"/>
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="15"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="20"/>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C34" s="1"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="15"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="20"/>
     </row>
     <row r="35" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C35" s="1"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="15"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="20"/>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C36" s="1"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="15"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="20"/>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C37" s="1"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="15"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="20"/>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C38" s="1"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="15"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="20"/>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C39" s="1"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="15"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B2:V2"/>
-    <mergeCell ref="D30:H30"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="D31:H31"/>
-    <mergeCell ref="D32:H32"/>
+    <mergeCell ref="D35:H35"/>
+    <mergeCell ref="D36:H36"/>
+    <mergeCell ref="D37:H37"/>
+    <mergeCell ref="D38:H38"/>
+    <mergeCell ref="D39:H39"/>
     <mergeCell ref="D33:H33"/>
     <mergeCell ref="D34:H34"/>
     <mergeCell ref="D28:H28"/>
@@ -1021,11 +1021,11 @@
     <mergeCell ref="D25:H25"/>
     <mergeCell ref="D26:H26"/>
     <mergeCell ref="D27:H27"/>
-    <mergeCell ref="D35:H35"/>
-    <mergeCell ref="D36:H36"/>
-    <mergeCell ref="D37:H37"/>
-    <mergeCell ref="D38:H38"/>
-    <mergeCell ref="D39:H39"/>
+    <mergeCell ref="B2:V2"/>
+    <mergeCell ref="D30:H30"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="D31:H31"/>
+    <mergeCell ref="D32:H32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1043,29 +1043,29 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="19"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="17"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>

</xml_diff>